<commit_message>
Fixing excel download logic
</commit_message>
<xml_diff>
--- a/backend/ExpenseData.xlsx
+++ b/backend/ExpenseData.xlsx
@@ -64,9 +64,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,69 +397,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Category</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Amount</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Date</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Car Service</v>
-      </c>
-      <c r="B2">
-        <v>4999</v>
-      </c>
-      <c r="C2" s="1">
-        <v>45960.22928240741</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Grocery</v>
-      </c>
-      <c r="B3">
-        <v>2400</v>
-      </c>
-      <c r="C3" s="1">
-        <v>45938.75355079861</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Shopping</v>
-      </c>
-      <c r="B4">
-        <v>4800</v>
-      </c>
-      <c r="C4" s="1">
-        <v>45938.75355079861</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Petrol</v>
-      </c>
-      <c r="B5">
-        <v>800</v>
-      </c>
-      <c r="C5" s="1">
-        <v>45938.75355079861</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>